<commit_message>
Updates: jwt cookies storage , UI contract details (gif added)
</commit_message>
<xml_diff>
--- a/ClientAstree/Words.xlsx
+++ b/ClientAstree/Words.xlsx
@@ -12,9 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>bad</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
 </sst>
 </file>
@@ -61,7 +67,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -72,6 +78,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>